<commit_message>
use F1 Score when filting features
</commit_message>
<xml_diff>
--- a/Features/相关性.xlsx
+++ b/Features/相关性.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="label_1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="181">
   <si>
     <t>column</t>
   </si>
@@ -571,6 +571,10 @@
   </si>
   <si>
     <t>IV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>equity</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -950,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1118,7 +1122,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="B12">
         <v>-0.1196</v>
@@ -13404,7 +13408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>